<commit_message>
Fix wrong referrals inside the excel table calculations for the D139 and D149 sensors
</commit_message>
<xml_diff>
--- a/sensor_table_logan.xlsx
+++ b/sensor_table_logan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
@@ -508,7 +508,7 @@
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -538,12 +538,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -691,7 +685,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -844,15 +838,15 @@
   </sheetPr>
   <dimension ref="A1:AZ203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="V14" activeCellId="0" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -1599,11 +1593,11 @@
         <v>83</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <f aca="false">(D6-C6)/(O6-N6)</f>
-        <v>625000</v>
+        <f aca="false">(D6-C6)/(H6-G6)</f>
+        <v>1249.00079936051</v>
       </c>
       <c r="R6" s="0" t="n">
-        <f aca="false">D6-(Q6*O6)</f>
+        <f aca="false">D6-(Q6*H6)</f>
         <v>-2500</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -1751,11 +1745,11 @@
         <v>83</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <f aca="false">(D7-C7)/(O7-N7)</f>
-        <v>625000</v>
+        <f aca="false">(D7-C7)/(H7-G7)</f>
+        <v>1249.00079936051</v>
       </c>
       <c r="R7" s="0" t="n">
-        <f aca="false">D7-(Q7*O7)</f>
+        <f aca="false">D7-(Q7*H7)</f>
         <v>-2500</v>
       </c>
       <c r="S7" s="1" t="s">
@@ -2631,11 +2625,11 @@
   </sheetPr>
   <dimension ref="A1:AU8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="X7" activeCellId="0" sqref="X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
@@ -2643,7 +2637,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.28"/>
@@ -3373,7 +3367,7 @@
       <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -4015,7 +4009,7 @@
   </sheetPr>
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -4023,7 +4017,7 @@
       <selection pane="bottomRight" activeCell="U25" activeCellId="0" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
@@ -4276,7 +4270,7 @@
         <v>58</v>
       </c>
       <c r="O3" s="0" t="n">
-        <f aca="false"> 0.1 + 0.4 + 0.05</f>
+        <f aca="false">0.1 + 0.4 + 0.05</f>
         <v>0.55</v>
       </c>
       <c r="P3" s="0" t="s">
@@ -4608,7 +4602,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
@@ -4853,7 +4847,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
   </cols>

</xml_diff>

<commit_message>
Fix further reference copy and paste errors inside the excel tables
</commit_message>
<xml_diff>
--- a/sensor_table_logan.xlsx
+++ b/sensor_table_logan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
@@ -838,7 +838,7 @@
   </sheetPr>
   <dimension ref="A1:AZ203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
@@ -846,7 +846,7 @@
       <selection pane="bottomRight" activeCell="V14" activeCellId="0" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -2625,11 +2625,11 @@
   </sheetPr>
   <dimension ref="A1:AU8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X7" activeCellId="0" sqref="X7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
@@ -2899,8 +2899,8 @@
         <v>0.000166666666666667</v>
       </c>
       <c r="N3" s="0" t="n">
-        <f aca="false">K3-(G3*M3)</f>
-        <v>0.0183333333333333</v>
+        <f aca="false">D3-(M3*G3)</f>
+        <v>0</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>58</v>
@@ -3040,8 +3040,8 @@
         <v>0.000166666666666667</v>
       </c>
       <c r="N4" s="0" t="n">
-        <f aca="false">K4-(G4*M4)</f>
-        <v>0.0183333333333333</v>
+        <f aca="false">D4-(M4*G4)</f>
+        <v>0</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>58</v>
@@ -3181,8 +3181,8 @@
         <v>0.000166666666666667</v>
       </c>
       <c r="N5" s="0" t="n">
-        <f aca="false">K5-(G5*M5)</f>
-        <v>0.0183333333333333</v>
+        <f aca="false">D5-(M5*G5)</f>
+        <v>0</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>58</v>
@@ -3367,7 +3367,7 @@
       <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -4017,7 +4017,7 @@
       <selection pane="bottomRight" activeCell="U25" activeCellId="0" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
@@ -4602,7 +4602,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
@@ -4847,7 +4847,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
   </cols>

</xml_diff>